<commit_message>
Update endo-learn/FoTOMRAEL with value lower than US value
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/FoTOMRAEL/Frac of Tech Outside Modeled Region Affecting Endo Learning.xlsx
+++ b/InputData/endo-learn/FoTOMRAEL/Frac of Tech Outside Modeled Region Affecting Endo Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\FoTOMRAEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\endo-learn\FoTOMRAEL (new)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D1A431-AF32-4B88-8B24-231C99A9E877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74499D8-21DB-4635-947A-2958D118F81E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="-14280" windowWidth="12840" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>About</t>
   </si>
@@ -48,9 +48,6 @@
     <t>FoTOMRAEL Fraction of Technology Outside Modeled Region Affecting Endogenous Learning</t>
   </si>
   <si>
-    <t>none specified</t>
-  </si>
-  <si>
     <t>Fraction</t>
   </si>
   <si>
@@ -103,6 +100,33 @@
   </si>
   <si>
     <t>onshore wind, offshore wind, solar PV, batteries, and CCS.</t>
+  </si>
+  <si>
+    <t>The US version of the EPS sets this value at 25%. Since the EU is a leader</t>
+  </si>
+  <si>
+    <t>in certain technologies, notably wind turbines, the value for the EU EPS</t>
+  </si>
+  <si>
+    <t>is set slightly lower at 20%.</t>
+  </si>
+  <si>
+    <t>US EPS</t>
+  </si>
+  <si>
+    <t>Version 3.1.3</t>
+  </si>
+  <si>
+    <t>European Commission</t>
+  </si>
+  <si>
+    <t>A technical case study on R&amp;D and technology spillovers of clean energy technologies</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/energy/sites/ener/files/documents/case_study_3_technical_analysis_spillovers.pdf</t>
+  </si>
+  <si>
+    <t>p. 17</t>
   </si>
 </sst>
 </file>
@@ -163,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -176,6 +200,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -458,122 +485,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="52.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B7" s="7">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{D38F335F-5491-4A43-814D-935109C3CD11}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -584,27 +655,29 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" customWidth="1"/>
+    <col min="1" max="1" width="46.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
       <c r="B2" s="5">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>